<commit_message>
New storage with support for DESIGN_MATRIX, v2025.01
</commit_message>
<xml_diff>
--- a/version-6/flow_design.xlsx
+++ b/version-6/flow_design.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KFLIK/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3141834C-1474-F248-9005-39E759643838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E78A26-CCB8-944F-A0A9-6A368223B3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23320" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23320" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="DefaultSheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>REAL</t>
   </si>
@@ -37,12 +38,15 @@
     <t xml:space="preserve">X_MID_PERMEABILITY
 </t>
   </si>
+  <si>
+    <t>dummy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -65,6 +69,12 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -212,7 +222,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -253,6 +263,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1387,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1620,4 +1633,27 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61DA990-E81E-2640-AC3A-87D4D89EFB97}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change to _number_ type for parameter
</commit_message>
<xml_diff>
--- a/version-6/flow_design.xlsx
+++ b/version-6/flow_design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KFLIK/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KFLIK/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E78A26-CCB8-944F-A0A9-6A368223B3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF75BDF-F6D6-8C4E-8DD6-5E7AC601BE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23320" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="1380" windowWidth="23320" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignSheet" sheetId="1" r:id="rId1"/>
@@ -21,18 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>REAL</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.9</t>
   </si>
   <si>
     <t xml:space="preserve">X_MID_PERMEABILITY
@@ -238,9 +229,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -248,9 +236,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -267,6 +252,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1400,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -1417,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1429,202 +1420,202 @@
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="8">
-        <v>1</v>
+      <c r="B3" s="14">
+        <v>0.1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>3</v>
+      <c r="B4" s="14">
+        <v>0.9</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
@@ -1639,15 +1630,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61DA990-E81E-2640-AC3A-87D4D89EFB97}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:2" ht="14">
-      <c r="A1" s="14" t="s">
-        <v>5</v>
+      <c r="A1" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="B1">
         <v>0</v>

</xml_diff>